<commit_message>
model based on SPY to see if it'll fit better to other equities
</commit_message>
<xml_diff>
--- a/Model Results 2.xlsx
+++ b/Model Results 2.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AAPL ML Perf" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SPY ML Perf" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="21">
   <si>
     <t xml:space="preserve">Lasso Regression</t>
   </si>
@@ -93,11 +94,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -116,18 +118,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -182,7 +172,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,24 +185,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -234,8 +236,8 @@
   </sheetPr>
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G58" activeCellId="0" sqref="G58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -276,161 +278,161 @@
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="5" t="n">
         <v>27.530294</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="5" t="n">
         <v>27.562171</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="5" t="n">
         <v>61.462004</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="5" t="n">
         <v>59.401281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="5" t="n">
         <v>60.961951</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="5" t="n">
         <v>60.734284</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="5" t="n">
         <v>23.648944</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="5" t="n">
         <v>24.350404</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>9.12736</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="6" t="n">
         <v>9.178331</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>56.541239</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="5" t="n">
         <v>58.015818</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="5" t="n">
         <v>9.013509</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="5" t="n">
         <v>9.013173</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="5" t="n">
         <v>54.917611</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="5" t="n">
         <v>42.312645</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="5" t="n">
         <v>54.328296</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="5" t="n">
         <v>54.314282</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="5" t="n">
         <v>61.462004</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="5" t="n">
         <v>59.401281</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="5" t="n">
         <v>123.717315</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="5" t="n">
         <v>123.368594</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="5" t="n">
         <v>23.648944</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="5" t="n">
         <v>24.350404</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="5" t="n">
         <v>17.890476</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="5" t="n">
         <v>17.927187</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="5" t="n">
         <v>57.801619</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="6" t="n">
         <v>54.47376</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="5" t="n">
         <v>18.290212</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="5" t="n">
         <v>18.290738</v>
       </c>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="5" t="n">
         <v>51.75437</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="5" t="n">
         <v>53.985356</v>
       </c>
     </row>
@@ -438,169 +440,169 @@
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="5" t="n">
         <v>0.027417</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="5" t="n">
         <v>0.126365</v>
       </c>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="5" t="n">
         <v>61.462004</v>
       </c>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="5" t="n">
         <v>59.401281</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="5" t="n">
         <v>0.005565</v>
       </c>
-      <c r="E12" s="6" t="n">
+      <c r="E12" s="5" t="n">
         <v>0.027345</v>
       </c>
-      <c r="F12" s="6" t="n">
+      <c r="F12" s="5" t="n">
         <v>23.648944</v>
       </c>
-      <c r="G12" s="6" t="n">
+      <c r="G12" s="5" t="n">
         <v>24.350404</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="5" t="n">
         <v>0.017533</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="5" t="n">
         <v>0.082571</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="6" t="n">
         <v>56.541239</v>
       </c>
-      <c r="G13" s="6" t="n">
+      <c r="G13" s="5" t="n">
         <v>58.015818</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="5" t="n">
         <v>0.015888</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E14" s="5" t="n">
         <v>0.070462</v>
       </c>
-      <c r="F14" s="6" t="n">
+      <c r="F14" s="5" t="n">
         <v>54.917611</v>
       </c>
-      <c r="G14" s="6" t="n">
+      <c r="G14" s="5" t="n">
         <v>42.312645</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="5" t="n">
         <v>0.025481</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="E15" s="5" t="n">
         <v>0.123415</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="5" t="n">
         <v>61.462004</v>
       </c>
-      <c r="G15" s="6" t="n">
+      <c r="G15" s="5" t="n">
         <v>59.401281</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="5" t="n">
         <v>0.005025</v>
       </c>
-      <c r="E16" s="6" t="n">
+      <c r="E16" s="5" t="n">
         <v>0.026894</v>
       </c>
-      <c r="F16" s="6" t="n">
+      <c r="F16" s="5" t="n">
         <v>23.648944</v>
       </c>
-      <c r="G16" s="6" t="n">
+      <c r="G16" s="5" t="n">
         <v>24.350404</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="6" t="n">
         <v>0.014529</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="6" t="n">
         <v>0.07799</v>
       </c>
-      <c r="F17" s="6" t="n">
+      <c r="F17" s="5" t="n">
         <v>57.521496</v>
       </c>
-      <c r="G17" s="7" t="n">
+      <c r="G17" s="6" t="n">
         <v>54.460597</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="6" t="n">
+      <c r="D18" s="5" t="n">
         <v>0.021479</v>
       </c>
-      <c r="E18" s="6" t="n">
+      <c r="E18" s="5" t="n">
         <v>0.08051</v>
       </c>
-      <c r="F18" s="6" t="n">
+      <c r="F18" s="5" t="n">
         <v>51.687269</v>
       </c>
-      <c r="G18" s="6" t="n">
+      <c r="G18" s="5" t="n">
         <v>53.972501</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -634,161 +636,161 @@
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="6" t="n">
+      <c r="D24" s="5" t="n">
         <v>0.020008</v>
       </c>
-      <c r="E24" s="6" t="n">
+      <c r="E24" s="5" t="n">
         <v>0.037439</v>
       </c>
-      <c r="F24" s="6" t="n">
+      <c r="F24" s="5" t="n">
         <v>12.975829</v>
       </c>
-      <c r="G24" s="6" t="n">
+      <c r="G24" s="5" t="n">
         <v>12.468895</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="6" t="n">
+      <c r="D25" s="5" t="n">
         <v>7.550736</v>
       </c>
-      <c r="E25" s="6" t="n">
+      <c r="E25" s="5" t="n">
         <v>7.240483</v>
       </c>
-      <c r="F25" s="6" t="n">
+      <c r="F25" s="5" t="n">
         <v>35.417361</v>
       </c>
-      <c r="G25" s="6" t="n">
+      <c r="G25" s="5" t="n">
         <v>34.345086</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="6" t="n">
+      <c r="D26" s="5" t="n">
         <v>0.014689</v>
       </c>
-      <c r="E26" s="6" t="n">
+      <c r="E26" s="5" t="n">
         <v>0.026369</v>
       </c>
-      <c r="F26" s="6" t="n">
+      <c r="F26" s="5" t="n">
         <v>11.401979</v>
       </c>
-      <c r="G26" s="7" t="n">
+      <c r="G26" s="6" t="n">
         <v>10.290046</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D27" s="5" t="n">
         <v>0.07438</v>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E27" s="5" t="n">
         <v>0.128783</v>
       </c>
-      <c r="F27" s="6" t="n">
+      <c r="F27" s="5" t="n">
         <v>90.43264</v>
       </c>
-      <c r="G27" s="6" t="n">
+      <c r="G27" s="5" t="n">
         <v>116.748852</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="6" t="n">
+      <c r="D28" s="5" t="n">
         <v>0.005641</v>
       </c>
-      <c r="E28" s="6" t="n">
+      <c r="E28" s="5" t="n">
         <v>0.017858</v>
       </c>
-      <c r="F28" s="6" t="n">
+      <c r="F28" s="5" t="n">
         <v>13.253872</v>
       </c>
-      <c r="G28" s="6" t="n">
+      <c r="G28" s="5" t="n">
         <v>10.415926</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="4"/>
       <c r="C29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="6" t="n">
+      <c r="D29" s="5" t="n">
         <v>6.163218</v>
       </c>
-      <c r="E29" s="6" t="n">
+      <c r="E29" s="5" t="n">
         <v>6.855677</v>
       </c>
-      <c r="F29" s="6" t="n">
+      <c r="F29" s="5" t="n">
         <v>36.405142</v>
       </c>
-      <c r="G29" s="6" t="n">
+      <c r="G29" s="5" t="n">
         <v>36.27584</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="7" t="n">
+      <c r="D30" s="6" t="n">
         <v>0.00353</v>
       </c>
-      <c r="E30" s="7" t="n">
+      <c r="E30" s="6" t="n">
         <v>0.012987</v>
       </c>
-      <c r="F30" s="7" t="n">
+      <c r="F30" s="6" t="n">
         <v>10.844997</v>
       </c>
-      <c r="G30" s="6" t="n">
+      <c r="G30" s="5" t="n">
         <v>10.591728</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="6" t="n">
+      <c r="D31" s="5" t="n">
         <v>0.017199</v>
       </c>
-      <c r="E31" s="6" t="n">
+      <c r="E31" s="5" t="n">
         <v>0.079194</v>
       </c>
-      <c r="F31" s="6" t="n">
+      <c r="F31" s="5" t="n">
         <v>67.404845</v>
       </c>
-      <c r="G31" s="6" t="n">
+      <c r="G31" s="5" t="n">
         <v>56.303109</v>
       </c>
     </row>
@@ -796,161 +798,161 @@
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="6" t="n">
+      <c r="D32" s="5" t="n">
         <v>0.020079</v>
       </c>
-      <c r="E32" s="6" t="n">
+      <c r="E32" s="5" t="n">
         <v>0.036673</v>
       </c>
-      <c r="F32" s="6" t="n">
+      <c r="F32" s="5" t="n">
         <v>58.527111</v>
       </c>
-      <c r="G32" s="6" t="n">
+      <c r="G32" s="5" t="n">
         <v>55.032623</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="4"/>
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="6" t="n">
+      <c r="D33" s="5" t="n">
         <v>7.233069</v>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E33" s="5" t="n">
         <v>9.064149</v>
       </c>
-      <c r="F33" s="6" t="n">
+      <c r="F33" s="5" t="n">
         <v>23.855048</v>
       </c>
-      <c r="G33" s="6" t="n">
+      <c r="G33" s="5" t="n">
         <v>25.982634</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="6" t="n">
+      <c r="D34" s="5" t="n">
         <v>0.014678</v>
       </c>
-      <c r="E34" s="6" t="n">
+      <c r="E34" s="5" t="n">
         <v>0.027818</v>
       </c>
-      <c r="F34" s="7" t="n">
+      <c r="F34" s="6" t="n">
         <v>49.504386</v>
       </c>
-      <c r="G34" s="7" t="n">
+      <c r="G34" s="6" t="n">
         <v>44.74414</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="4"/>
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="6" t="n">
+      <c r="D35" s="5" t="n">
         <v>0.071163</v>
       </c>
-      <c r="E35" s="6" t="n">
+      <c r="E35" s="5" t="n">
         <v>0.141436</v>
       </c>
-      <c r="F35" s="6" t="n">
+      <c r="F35" s="5" t="n">
         <v>82.508215</v>
       </c>
-      <c r="G35" s="6" t="n">
+      <c r="G35" s="5" t="n">
         <v>107.522642</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="6" t="n">
+      <c r="D36" s="5" t="n">
         <v>0.009818</v>
       </c>
-      <c r="E36" s="6" t="n">
+      <c r="E36" s="5" t="n">
         <v>0.040079</v>
       </c>
-      <c r="F36" s="6" t="n">
+      <c r="F36" s="5" t="n">
         <v>55.228393</v>
       </c>
-      <c r="G36" s="6" t="n">
+      <c r="G36" s="5" t="n">
         <v>54.899313</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="4"/>
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="6" t="n">
+      <c r="D37" s="5" t="n">
         <v>6.138481</v>
       </c>
-      <c r="E37" s="6" t="n">
+      <c r="E37" s="5" t="n">
         <v>6.876906</v>
       </c>
-      <c r="F37" s="6" t="n">
+      <c r="F37" s="5" t="n">
         <v>23.744145</v>
       </c>
-      <c r="G37" s="6" t="n">
+      <c r="G37" s="5" t="n">
         <v>26.847332</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="7" t="n">
+      <c r="D38" s="6" t="n">
         <v>0.004038</v>
       </c>
-      <c r="E38" s="7" t="n">
+      <c r="E38" s="6" t="n">
         <v>0.013244</v>
       </c>
-      <c r="F38" s="6" t="n">
+      <c r="F38" s="5" t="n">
         <v>49.804594</v>
       </c>
-      <c r="G38" s="6" t="n">
+      <c r="G38" s="5" t="n">
         <v>50.177182</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="6" t="n">
+      <c r="D39" s="5" t="n">
         <v>0.016825</v>
       </c>
-      <c r="E39" s="6" t="n">
+      <c r="E39" s="5" t="n">
         <v>0.075946</v>
       </c>
-      <c r="F39" s="6" t="n">
+      <c r="F39" s="5" t="n">
         <v>62.111085</v>
       </c>
-      <c r="G39" s="6" t="n">
+      <c r="G39" s="5" t="n">
         <v>53.367439</v>
       </c>
     </row>
@@ -980,113 +982,113 @@
       <c r="A44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="6" t="n">
+      <c r="D44" s="5" t="n">
         <v>65.528596</v>
       </c>
-      <c r="E44" s="6" t="n">
+      <c r="E44" s="5" t="n">
         <v>64.523397</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
+      <c r="B45" s="4"/>
       <c r="C45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="6" t="n">
+      <c r="D45" s="5" t="n">
         <v>50.519751</v>
       </c>
-      <c r="E45" s="6" t="n">
+      <c r="E45" s="5" t="n">
         <v>45.530146</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="7" t="n">
+      <c r="D46" s="6" t="n">
         <v>65.684575</v>
       </c>
-      <c r="E46" s="6" t="n">
+      <c r="E46" s="5" t="n">
         <v>64.090121</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
+      <c r="B47" s="4"/>
       <c r="C47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="6" t="n">
+      <c r="D47" s="5" t="n">
         <v>51.489951</v>
       </c>
-      <c r="E47" s="6" t="n">
+      <c r="E47" s="5" t="n">
         <v>53.776854</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="6" t="n">
+      <c r="D48" s="5" t="n">
         <v>65.164645</v>
       </c>
-      <c r="E48" s="6" t="n">
+      <c r="E48" s="5" t="n">
         <v>66.187175</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
-      <c r="B49" s="5"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="6" t="n">
+      <c r="D49" s="5" t="n">
         <v>50.45045</v>
       </c>
-      <c r="E49" s="6" t="n">
+      <c r="E49" s="5" t="n">
         <v>52.598753</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="6" t="n">
+      <c r="D50" s="5" t="n">
         <v>64.662045</v>
       </c>
-      <c r="E50" s="7" t="n">
+      <c r="E50" s="6" t="n">
         <v>67.157712</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
-      <c r="B51" s="5"/>
+      <c r="B51" s="4"/>
       <c r="C51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="6" t="n">
+      <c r="D51" s="5" t="n">
         <v>51.628552</v>
       </c>
-      <c r="E51" s="6" t="n">
+      <c r="E51" s="5" t="n">
         <v>57.033957</v>
       </c>
     </row>
@@ -1094,113 +1096,113 @@
       <c r="A52" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="6" t="n">
+      <c r="D52" s="5" t="n">
         <v>54.020797</v>
       </c>
-      <c r="E52" s="6" t="n">
+      <c r="E52" s="5" t="n">
         <v>58.838821</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
-      <c r="B53" s="5"/>
+      <c r="B53" s="4"/>
       <c r="C53" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="6" t="n">
+      <c r="D53" s="5" t="n">
         <v>51.905752</v>
       </c>
-      <c r="E53" s="6" t="n">
+      <c r="E53" s="5" t="n">
         <v>45.599446</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="7" t="n">
+      <c r="D54" s="6" t="n">
         <v>54.07279</v>
       </c>
-      <c r="E54" s="6" t="n">
+      <c r="E54" s="5" t="n">
         <v>88.110919</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
-      <c r="B55" s="5"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="6" t="n">
+      <c r="D55" s="5" t="n">
         <v>52.390852</v>
       </c>
-      <c r="E55" s="6" t="n">
+      <c r="E55" s="5" t="n">
         <v>54.400554</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="6" t="n">
+      <c r="D56" s="5" t="n">
         <v>53.639515</v>
       </c>
-      <c r="E56" s="7" t="n">
+      <c r="E56" s="6" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
+      <c r="B57" s="4"/>
       <c r="C57" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="6" t="n">
+      <c r="D57" s="5" t="n">
         <v>52.113652</v>
       </c>
-      <c r="E57" s="6" t="n">
+      <c r="E57" s="5" t="n">
         <v>54.192654</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="6" t="n">
+      <c r="D58" s="5" t="n">
         <v>53.691508</v>
       </c>
-      <c r="E58" s="6" t="n">
+      <c r="E58" s="5" t="n">
         <v>99.566724</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
-      <c r="B59" s="5"/>
+      <c r="B59" s="4"/>
       <c r="C59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="6" t="n">
+      <c r="D59" s="5" t="n">
         <v>52.945253</v>
       </c>
-      <c r="E59" s="6" t="n">
+      <c r="E59" s="5" t="n">
         <v>60.49896</v>
       </c>
     </row>
@@ -1221,34 +1223,34 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="6" t="n">
+      <c r="D63" s="5" t="n">
         <v>0.00518367125261209</v>
       </c>
-      <c r="E63" s="6" t="n">
+      <c r="E63" s="5" t="n">
         <v>0.000966864827828244</v>
       </c>
-      <c r="F63" s="6" t="n">
+      <c r="F63" s="5" t="n">
         <v>0.558909090909091</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="5"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D64" s="6" t="n">
+      <c r="D64" s="5" t="n">
         <v>0.0224159558116534</v>
       </c>
-      <c r="E64" s="6" t="n">
+      <c r="E64" s="5" t="n">
         <v>0.000210796723055422</v>
       </c>
-      <c r="F64" s="6" t="n">
+      <c r="F64" s="5" t="n">
         <v>0.51</v>
       </c>
     </row>
@@ -1294,4 +1296,1407 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N64"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.003356</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.013741</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>36.911438</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>30.663134</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.001142</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.005471</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>11.733432</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>11.17065</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.002735</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.011924</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>29.86762</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>26.368235</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.003223</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.010884</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>34.085833</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>22.927536</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.003358</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.013679</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>36.926949</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>30.522251</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.001139</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.005384</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>11.725034</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>10.998997</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0.002849</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.011529</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>22.615644</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>24.203148</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.002773</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.01229</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>-58.939518</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>32.246054</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>0.021175</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>0.021564</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>8.749728</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>6.243914</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>4.707592</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>4.531282</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>15.846539</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>20.040556</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.020948</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.023331</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>6.134662</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>5.175591</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.11033</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.11974</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>37.591602</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>26.008136</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.00077</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.002467</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>7.975724</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>5.999654</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>2.2488</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>2.309355</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>13.239699</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>13.512031</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>0.000626</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>0.002115</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>4.601719</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>4.726889</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.003302</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.011972</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>-67.510894</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>31.878425</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.021175</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.021564</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>8.749728</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>6.243914</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>4.707592</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>4.531282</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>15.846539</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>20.040556</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="5" t="n">
+        <v>0.020948</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>0.023331</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>6.134662</v>
+      </c>
+      <c r="G26" s="5" t="n">
+        <v>5.175591</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>0.11033</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>0.11974</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>37.591602</v>
+      </c>
+      <c r="G27" s="5" t="n">
+        <v>26.008136</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="5" t="n">
+        <v>0.00077</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>0.002467</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>7.975724</v>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>5.999654</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>2.2488</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>2.309355</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>13.239699</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>13.512031</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="5" t="n">
+        <v>0.000626</v>
+      </c>
+      <c r="E30" s="5" t="n">
+        <v>0.002115</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>4.601719</v>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>4.726889</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>0.003302</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>0.011972</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>-67.510894</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>31.878425</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>0.01978</v>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>0.021266</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>32.868408</v>
+      </c>
+      <c r="G32" s="5" t="n">
+        <v>27.690727</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5" t="n">
+        <v>4.562385</v>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>4.593628</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>11.433277</v>
+      </c>
+      <c r="G33" s="5" t="n">
+        <v>10.387701</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="5" t="n">
+        <v>0.022056</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>0.022087</v>
+      </c>
+      <c r="F34" s="5" t="n">
+        <v>26.807339</v>
+      </c>
+      <c r="G34" s="5" t="n">
+        <v>23.859003</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="5" t="n">
+        <v>0.114683</v>
+      </c>
+      <c r="E35" s="5" t="n">
+        <v>0.119282</v>
+      </c>
+      <c r="F35" s="5" t="n">
+        <v>34.585136</v>
+      </c>
+      <c r="G35" s="5" t="n">
+        <v>23.696645</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="5" t="n">
+        <v>0.001539</v>
+      </c>
+      <c r="E36" s="5" t="n">
+        <v>0.00559</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>32.867543</v>
+      </c>
+      <c r="G36" s="5" t="n">
+        <v>26.898148</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="5" t="n">
+        <v>2.262511</v>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>2.294137</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>11.307823</v>
+      </c>
+      <c r="G37" s="5" t="n">
+        <v>10.430583</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="5" t="n">
+        <v>0.001263</v>
+      </c>
+      <c r="E38" s="5" t="n">
+        <v>0.00207</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>19.646285</v>
+      </c>
+      <c r="G38" s="5" t="n">
+        <v>21.668667</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="5" t="n">
+        <v>0.003194</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>0.012146</v>
+      </c>
+      <c r="F39" s="5" t="n">
+        <v>-60.326193</v>
+      </c>
+      <c r="G39" s="5" t="n">
+        <v>31.505395</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="7"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="7"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="7"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="7"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="5" t="n">
+        <v>63.357296</v>
+      </c>
+      <c r="E44" s="5" t="n">
+        <v>66.232757</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="7"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="5" t="n">
+        <v>52.602953</v>
+      </c>
+      <c r="E45" s="5" t="n">
+        <v>54.001554</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="7"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <v>64.056732</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v>65.358461</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="7"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="5" t="n">
+        <v>55.633256</v>
+      </c>
+      <c r="E47" s="5" t="n">
+        <v>56.876457</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="7"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="5" t="n">
+        <v>65.125316</v>
+      </c>
+      <c r="E48" s="5" t="n">
+        <v>67.767632</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="7"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="5" t="n">
+        <v>51.204351</v>
+      </c>
+      <c r="E49" s="5" t="n">
+        <v>45.609946</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="7"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="5" t="n">
+        <v>65.319604</v>
+      </c>
+      <c r="E50" s="5" t="n">
+        <v>67.379056</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="7"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="5" t="n">
+        <v>53.302253</v>
+      </c>
+      <c r="E51" s="5" t="n">
+        <v>62.082362</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="7"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="5" t="n">
+        <v>54.866913</v>
+      </c>
+      <c r="E52" s="5" t="n">
+        <v>61.103555</v>
+      </c>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="7"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="5" t="n">
+        <v>55.322455</v>
+      </c>
+      <c r="E53" s="5" t="n">
+        <v>60.683761</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="7"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="5" t="n">
+        <v>55.857781</v>
+      </c>
+      <c r="E54" s="5" t="n">
+        <v>62.483</v>
+      </c>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="5" t="n">
+        <v>54.390054</v>
+      </c>
+      <c r="E55" s="5" t="n">
+        <v>56.177156</v>
+      </c>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="5" t="n">
+        <v>84.923256</v>
+      </c>
+      <c r="E56" s="5" t="n">
+        <v>94.423936</v>
+      </c>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="5" t="n">
+        <v>45.843046</v>
+      </c>
+      <c r="E57" s="5" t="n">
+        <v>48.717949</v>
+      </c>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="5" t="n">
+        <v>58.500097</v>
+      </c>
+      <c r="E58" s="5" t="n">
+        <v>91.898193</v>
+      </c>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="5" t="n">
+        <v>54.001554</v>
+      </c>
+      <c r="E59" s="5" t="n">
+        <v>62.703963</v>
+      </c>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B63" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="5" t="n">
+        <v>0.0196587165125582</v>
+      </c>
+      <c r="E63" s="5" t="n">
+        <v>0.000154372042423037</v>
+      </c>
+      <c r="F63" s="5" t="n">
+        <v>0.74078431372549</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="4"/>
+      <c r="C64" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="5" t="n">
+        <v>0.444477006642558</v>
+      </c>
+      <c r="E64" s="5" t="n">
+        <v>6.65334057425316E-005</v>
+      </c>
+      <c r="F64" s="5" t="n">
+        <v>0.494166666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B63:B64"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
introducing sentdex's version of LSTM into my analysis (introduction)
</commit_message>
<xml_diff>
--- a/Model Results 2.xlsx
+++ b/Model Results 2.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AAPL ML Perf" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SPY ML Perf" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Model Performance" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="36">
   <si>
     <t xml:space="preserve">Lasso Regression</t>
   </si>
@@ -84,15 +85,61 @@
   </si>
   <si>
     <t xml:space="preserve">LSTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPY Model Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPY train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPY test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPY Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAPL Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HD Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMZN Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VXX Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAPL Model Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAPL train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAPL test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AALP Updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -172,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,6 +262,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1305,8 +1360,8 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1992,16 +2047,16 @@
       <c r="C30" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="D30" s="6" t="n">
         <v>0.000626</v>
       </c>
-      <c r="E30" s="5" t="n">
+      <c r="E30" s="6" t="n">
         <v>0.002115</v>
       </c>
-      <c r="F30" s="5" t="n">
+      <c r="F30" s="6" t="n">
         <v>4.601719</v>
       </c>
-      <c r="G30" s="5" t="n">
+      <c r="G30" s="6" t="n">
         <v>4.726889</v>
       </c>
       <c r="H30" s="3"/>
@@ -2194,10 +2249,10 @@
       <c r="C38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="5" t="n">
+      <c r="D38" s="6" t="n">
         <v>0.001263</v>
       </c>
-      <c r="E38" s="5" t="n">
+      <c r="E38" s="6" t="n">
         <v>0.00207</v>
       </c>
       <c r="F38" s="5" t="n">
@@ -2542,10 +2597,10 @@
       <c r="C56" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="5" t="n">
+      <c r="D56" s="6" t="n">
         <v>84.923256</v>
       </c>
-      <c r="E56" s="5" t="n">
+      <c r="E56" s="6" t="n">
         <v>94.423936</v>
       </c>
       <c r="F56" s="10"/>
@@ -2635,7 +2690,7 @@
       <c r="D63" s="5" t="n">
         <v>0.0196587165125582</v>
       </c>
-      <c r="E63" s="5" t="n">
+      <c r="E63" s="6" t="n">
         <v>0.000154372042423037</v>
       </c>
       <c r="F63" s="5" t="n">
@@ -2650,7 +2705,7 @@
       <c r="D64" s="5" t="n">
         <v>0.444477006642558</v>
       </c>
-      <c r="E64" s="5" t="n">
+      <c r="E64" s="6" t="n">
         <v>6.65334057425316E-005</v>
       </c>
       <c r="F64" s="5" t="n">
@@ -2699,4 +2754,422 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3"/>
+      <c r="C2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>6E-006</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>2.1E-005</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0.378107</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>0.049637</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>0.849233</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>0.944239</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11"/>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>2.8E-005</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>0.000106</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0.140552</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0.196893</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>0.45843</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>0.487179</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="12" t="n">
+        <v>1.073274E-005</v>
+      </c>
+      <c r="D6" s="12" t="n">
+        <v>3.767846E-005</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>0.318148</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>0.318148</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>0.768336</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <v>0.850829</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+      <c r="B7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>2.166155</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>2.180536</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>0.525623</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>0.628332</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>0.525623</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>0.542105</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>0.224574</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0.227192</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>0.429825</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>0.447163</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>0.526009</v>
+      </c>
+      <c r="H8" s="8" t="n">
+        <v>0.541228</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11"/>
+      <c r="B9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>0.000998</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>0.001475</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>0.297111</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>0.449101</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>0.498738</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>0.479192</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+      <c r="B10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>0.093649</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0.093773</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>0.850402</v>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>0.7661</v>
+      </c>
+      <c r="G10" s="8" t="n">
+        <v>0.491424</v>
+      </c>
+      <c r="H10" s="8" t="n">
+        <v>0.510439</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+      <c r="B11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>0.970598</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>0.958418</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>-4.20709</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>-0.887993</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <v>0.549627</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <v>0.51282</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <v>3.7E-005</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>0.000125</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0.654767</v>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>0.110388</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>0.545234</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11"/>
+      <c r="B14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>0.000196</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0.000755</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>0.22136</v>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>0.594891</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <v>0.52183</v>
+      </c>
+      <c r="H14" s="8" t="n">
+        <v>0.541927</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11"/>
+      <c r="B15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="12" t="n">
+        <v>6.64E-005</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <v>0.00024</v>
+      </c>
+      <c r="E15" s="8" t="n">
+        <v>0.608699</v>
+      </c>
+      <c r="F15" s="8" t="n">
+        <v>0.216528</v>
+      </c>
+      <c r="G15" s="8" t="n">
+        <v>0.540997</v>
+      </c>
+      <c r="H15" s="8" t="n">
+        <v>0.908033</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="8" t="n">
+        <v>0.000526</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <v>0.000693</v>
+      </c>
+      <c r="E16" s="8" t="n">
+        <v>0.411881</v>
+      </c>
+      <c r="F16" s="8" t="n">
+        <v>0.456691</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <v>0.543518</v>
+      </c>
+      <c r="H16" s="8" t="n">
+        <v>0.497979</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11"/>
+      <c r="B17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>0.000174</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <v>0.000911</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>0.457377</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>0.567149</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>0.531401</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>0.504644</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11"/>
+      <c r="B18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v>1.128718</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v>1.110198</v>
+      </c>
+      <c r="E18" s="8" t="n">
+        <v>-4.37429</v>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v>-0.952606</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>0.447773</v>
+      </c>
+      <c r="H18" s="8" t="n">
+        <v>0.544319</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A13:A18"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
getting sentdex's code to work, and view visualization on tensorboard
</commit_message>
<xml_diff>
--- a/Model Results 2.xlsx
+++ b/Model Results 2.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="AAPL ML Perf" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SPY ML Perf" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Model Performance" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Optimized Model Performance" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -292,7 +292,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
+      <selection pane="topLeft" activeCell="D43" activeCellId="1" sqref="H7:H8 D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1361,7 +1361,7 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
+      <selection pane="topLeft" activeCell="L30" activeCellId="1" sqref="H7:H8 L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2764,7 +2764,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>